<commit_message>
misc edits to docs
</commit_message>
<xml_diff>
--- a/docs/Dastruct - 2022-07-18.xlsx
+++ b/docs/Dastruct - 2022-07-18.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/everett/Codes/Projects/Work/Workforce/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14283E0-2318-E141-B365-F1BF54EB6FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D003C3-89B7-4442-A97B-A2B8E145FDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="400" yWindow="2480" windowWidth="30420" windowHeight="17680" activeTab="2" xr2:uid="{208C766E-858D-E64E-9905-BF5B2B6B0DAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Infrastructure" sheetId="3" r:id="rId1"/>
     <sheet name="Authentication" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="Customer Contact" sheetId="4" r:id="rId3"/>
     <sheet name="Configuration" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="96">
   <si>
     <t>App</t>
   </si>
@@ -128,6 +128,204 @@
   </si>
   <si>
     <t>Master files</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>text() = json</t>
+  </si>
+  <si>
+    <t>tin</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>contact_type(website, landline, mobile, fax, email, etc...), value</t>
+  </si>
+  <si>
+    <t>ref_no</t>
+  </si>
+  <si>
+    <t>tb_wf_mf_entity</t>
+  </si>
+  <si>
+    <t>entity_id, …..</t>
+  </si>
+  <si>
+    <t>hospital, doctor, office, etc…</t>
+  </si>
+  <si>
+    <t>tb_wf_mf_entity_relationship</t>
+  </si>
+  <si>
+    <t>pk</t>
+  </si>
+  <si>
+    <t>primary_entity_id</t>
+  </si>
+  <si>
+    <t>secondary_entity_id</t>
+  </si>
+  <si>
+    <t>fk</t>
+  </si>
+  <si>
+    <t>(hospital, office)</t>
+  </si>
+  <si>
+    <t>(person, i.e. doctors, office staff, etc…)</t>
+  </si>
+  <si>
+    <t>tb_wf_mf_entity_type</t>
+  </si>
+  <si>
+    <t>entity_type_id:</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>primary / secondary</t>
+  </si>
+  <si>
+    <t>primary : hospital, office</t>
+  </si>
+  <si>
+    <t>secondary : person, i.e. docotors, office staff,</t>
+  </si>
+  <si>
+    <t>entity_relationship_ids</t>
+  </si>
+  <si>
+    <t>boss_id</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>fk, nullable</t>
+  </si>
+  <si>
+    <t>Everett</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>Robin</t>
+  </si>
+  <si>
+    <t>Asher</t>
+  </si>
+  <si>
+    <t>Debie</t>
+  </si>
+  <si>
+    <t>tb_wf_mf_territory</t>
+  </si>
+  <si>
+    <t>Winterpine</t>
+  </si>
+  <si>
+    <t>Mags Department</t>
+  </si>
+  <si>
+    <t>Tint Department</t>
+  </si>
+  <si>
+    <t>Luzon</t>
+  </si>
+  <si>
+    <t>Vizayas</t>
+  </si>
+  <si>
+    <t>Mindanao</t>
+  </si>
+  <si>
+    <t>Metro Manila</t>
+  </si>
+  <si>
+    <t>North Luzon</t>
+  </si>
+  <si>
+    <t>South Luzon</t>
+  </si>
+  <si>
+    <t>QC</t>
+  </si>
+  <si>
+    <t>Manila, Kalookan</t>
+  </si>
+  <si>
+    <t>Pasig</t>
+  </si>
+  <si>
+    <t>&lt;---- Territory</t>
+  </si>
+  <si>
+    <t>(Business Unit, Area)</t>
+  </si>
+  <si>
+    <t>Tint, Luzon - MM, QC</t>
+  </si>
+  <si>
+    <t>Tint, Luzon - MM, Maynila, Kalook</t>
+  </si>
+  <si>
+    <t>Tint, Luzon - MM, Pasig</t>
+  </si>
+  <si>
+    <t>--&gt;</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>business_unit</t>
+  </si>
+  <si>
+    <t>varchar(100</t>
+  </si>
+  <si>
+    <t>varchar(30)</t>
+  </si>
+  <si>
+    <t>tb_sys_mf_user_territory</t>
+  </si>
+  <si>
+    <t>territory_id</t>
+  </si>
+  <si>
+    <t>tb_wf_mf_entity_address</t>
+  </si>
+  <si>
+    <t>brgy</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>province</t>
+  </si>
+  <si>
+    <t>tb_wf_mf_entity_address_territory</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>entity_id</t>
+  </si>
+  <si>
+    <t>entity_address_id</t>
   </si>
 </sst>
 </file>
@@ -2862,10 +3060,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F23E5E3-6637-B241-A3A6-FB16A95A50A2}">
-  <dimension ref="D4:AY25"/>
+  <dimension ref="D4:BE40"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="157" workbookViewId="0">
-      <selection activeCell="AB31" sqref="AB31"/>
+    <sheetView topLeftCell="O1" zoomScale="129" workbookViewId="0">
+      <selection activeCell="AF36" sqref="AF36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2961,13 +3159,19 @@
     </row>
     <row r="12" spans="4:51" x14ac:dyDescent="0.2">
       <c r="AM12" t="s">
-        <v>9</v>
+        <v>55</v>
+      </c>
+      <c r="AP12" t="s">
+        <v>57</v>
       </c>
       <c r="AY12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="4:51" x14ac:dyDescent="0.2">
+      <c r="AM13" t="s">
+        <v>9</v>
+      </c>
       <c r="AY13" t="s">
         <v>17</v>
       </c>
@@ -2981,44 +3185,175 @@
       <c r="W15" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="AL15" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="4:51" x14ac:dyDescent="0.2">
+      <c r="AM16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="23:57" x14ac:dyDescent="0.2">
       <c r="W17" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="AM17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="23:57" x14ac:dyDescent="0.2">
       <c r="W18" s="4"/>
-    </row>
-    <row r="20" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="AM18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="23:57" x14ac:dyDescent="0.2">
       <c r="W20" s="7" t="s">
         <v>14</v>
       </c>
       <c r="X20" s="7"/>
-    </row>
-    <row r="21" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="AL20" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="23:57" x14ac:dyDescent="0.2">
       <c r="W21" s="7"/>
       <c r="X21" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="AM21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="23:57" x14ac:dyDescent="0.2">
       <c r="W22" s="7"/>
       <c r="X22" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="AN22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="23:57" x14ac:dyDescent="0.2">
       <c r="W23" s="7"/>
       <c r="X23" s="7"/>
-    </row>
-    <row r="24" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="AO23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="23:57" x14ac:dyDescent="0.2">
       <c r="W24" s="7"/>
       <c r="X24" s="7"/>
-    </row>
-    <row r="25" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="AP24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="23:57" x14ac:dyDescent="0.2">
       <c r="W25" s="7"/>
       <c r="X25" s="7"/>
+    </row>
+    <row r="28" spans="23:57" x14ac:dyDescent="0.2">
+      <c r="AO28" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="23:57" x14ac:dyDescent="0.2">
+      <c r="AP29" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="23:57" x14ac:dyDescent="0.2">
+      <c r="AP30" s="5"/>
+      <c r="AQ30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="23:57" x14ac:dyDescent="0.2">
+      <c r="AP31" s="5"/>
+      <c r="AR31" t="s">
+        <v>70</v>
+      </c>
+      <c r="BE31" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="23:57" x14ac:dyDescent="0.2">
+      <c r="AP32" s="5"/>
+      <c r="AS32" t="s">
+        <v>73</v>
+      </c>
+      <c r="AZ32" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD32" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="BE32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="42:57" x14ac:dyDescent="0.2">
+      <c r="AP33" s="5"/>
+      <c r="AS33" t="s">
+        <v>74</v>
+      </c>
+      <c r="AZ33" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="BE33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="42:57" x14ac:dyDescent="0.2">
+      <c r="AP34" s="5"/>
+      <c r="AS34" t="s">
+        <v>75</v>
+      </c>
+      <c r="AZ34" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD34" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="BE34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="42:57" x14ac:dyDescent="0.2">
+      <c r="AP35" s="5"/>
+      <c r="AR35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="42:57" x14ac:dyDescent="0.2">
+      <c r="AP36" s="5"/>
+      <c r="AR36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="42:57" x14ac:dyDescent="0.2">
+      <c r="AP37" s="5"/>
+      <c r="AQ37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="42:57" x14ac:dyDescent="0.2">
+      <c r="AP38" s="5"/>
+      <c r="AQ38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="42:57" x14ac:dyDescent="0.2">
+      <c r="AP39" s="5"/>
+    </row>
+    <row r="40" spans="42:57" x14ac:dyDescent="0.2">
+      <c r="AP40" s="5" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3032,14 +3367,291 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46123D7F-0722-2B46-ABF8-1C1A7A5D661F}">
-  <dimension ref="A1"/>
+  <dimension ref="E3:I58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E3" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E5" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E18" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>94</v>
+      </c>
+      <c r="G20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E27" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>95</v>
+      </c>
+      <c r="G28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="F29" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="F30" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E35" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="F36" t="s">
+        <v>5</v>
+      </c>
+      <c r="G36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="F37" t="s">
+        <v>43</v>
+      </c>
+      <c r="G37" t="s">
+        <v>45</v>
+      </c>
+      <c r="H37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="F38" t="s">
+        <v>44</v>
+      </c>
+      <c r="G38" t="s">
+        <v>45</v>
+      </c>
+      <c r="H38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E44" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="F45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="F46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="F47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="F48" t="s">
+        <v>50</v>
+      </c>
+      <c r="H48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="H49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="H50" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E53" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="F54" t="s">
+        <v>5</v>
+      </c>
+      <c r="I54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="F55" t="s">
+        <v>6</v>
+      </c>
+      <c r="I55" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="F56" t="s">
+        <v>7</v>
+      </c>
+      <c r="I56" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="57" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="F57" t="s">
+        <v>82</v>
+      </c>
+      <c r="I57" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="58" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="F58" t="s">
+        <v>83</v>
+      </c>
+      <c r="I58" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>